<commit_message>
Refactor: Replace xlsx with ExcelJS for XLSX handling
This commit replaces the `xlsx` library with `ExcelJS` for reading and writing Excel files. This change improves compatibility and performance, especially in browser environments. The README has been updated to reflect this change and add a security note regarding dependency management.

Co-authored-by: magnusbakken <magnusbakken@gmail.com>
</commit_message>
<xml_diff>
--- a/src/utils/__tests__/fixtures/case1/expected-output.xlsx
+++ b/src/utils/__tests__/fixtures/case1/expected-output.xlsx
@@ -1,48 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Import" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Import" state="visible" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+  <si>
+    <t>LineNum</t>
+  </si>
+  <si>
+    <t>ProjectDataAreaId</t>
+  </si>
+  <si>
+    <t>ProjId</t>
+  </si>
+  <si>
+    <t>ACTIVITYNUMBER</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>NO01</t>
+  </si>
+  <si>
+    <t>051038</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>-3.75</t>
+  </si>
+  <si>
+    <t>-4.75</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="#,##0"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,13 +113,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,183 +452,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>LineNum</v>
-      </c>
-      <c r="B1" t="str">
-        <v>ProjectDataAreaId</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ProjId</v>
-      </c>
-      <c r="D1" t="str">
-        <v>ACTIVITYNUMBER</v>
-      </c>
-      <c r="E1" t="str">
-        <v>HOURS</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Hours2_</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Hours3_</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Hours4_</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Hours5_</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Hours6_</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Hours7_</v>
-      </c>
-      <c r="L1" t="str">
-        <v>EXTERNALCOMMENTS</v>
-      </c>
-      <c r="M1" t="str">
-        <v>ExternalComments2_</v>
-      </c>
-      <c r="N1" t="str">
-        <v>ExternalComments3_</v>
-      </c>
-      <c r="O1" t="str">
-        <v>ExternalComments4_</v>
-      </c>
-      <c r="P1" t="str">
-        <v>ExternalComments5_</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>ExternalComments6_</v>
-      </c>
-      <c r="R1" t="str">
-        <v>ExternalComments7_</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>1.0000000000000000</v>
-      </c>
-      <c r="B2" t="str">
-        <v>110</v>
-      </c>
-      <c r="C2" t="str">
-        <v>11011127</v>
-      </c>
-      <c r="D2" t="str">
-        <v>A110015929</v>
-      </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2">
-        <v>7.5</v>
-      </c>
-      <c r="G2">
-        <v>7.5</v>
-      </c>
-      <c r="H2">
-        <v>9.5</v>
-      </c>
-      <c r="I2">
-        <v>7.5</v>
-      </c>
-      <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="M2" t="str">
-        <v>Development</v>
-      </c>
-      <c r="N2" t="str">
-        <v>Development</v>
-      </c>
-      <c r="O2" t="str">
-        <v>Development</v>
-      </c>
-      <c r="P2" t="str">
-        <v>Development</v>
-      </c>
-      <c r="Q2" t="str">
-        <v/>
-      </c>
-      <c r="R2" t="str">
-        <v/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2.0000000000000000</v>
-      </c>
-      <c r="B3" t="str">
-        <v>110</v>
-      </c>
-      <c r="C3" t="str">
-        <v>11011127</v>
-      </c>
-      <c r="D3" t="str">
-        <v>A110015932</v>
-      </c>
-      <c r="E3" t="str">
-        <v/>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="G3">
-        <v>0.5</v>
-      </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-      <c r="M3" t="str">
-        <v>Lunsj</v>
-      </c>
-      <c r="N3" t="str">
-        <v>Lunsj</v>
-      </c>
-      <c r="O3" t="str">
-        <v>Lunsj</v>
-      </c>
-      <c r="P3" t="str">
-        <v>Lunsj</v>
-      </c>
-      <c r="Q3" t="str">
-        <v/>
-      </c>
-      <c r="R3" t="str">
-        <v/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R3"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>